<commit_message>
break times changed to TTh 3-5, five day lunch activity added
</commit_message>
<xml_diff>
--- a/RoomNumbers.xlsx
+++ b/RoomNumbers.xlsx
@@ -369,8 +369,8 @@
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="A10:B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -792,7 +792,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>1</v>
@@ -883,7 +883,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="1" sqref="A10:B10 B15"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
rooms updated. consecutive classes get same rooms
</commit_message>
<xml_diff>
--- a/RoomNumbers.xlsx
+++ b/RoomNumbers.xlsx
@@ -25,15 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t xml:space="preserve">Room</t>
   </si>
   <si>
-    <t xml:space="preserve">Seating Capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biometric</t>
+    <t xml:space="preserve">Capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biometric?</t>
   </si>
   <si>
     <t xml:space="preserve">A216</t>
@@ -132,6 +132,9 @@
     <t xml:space="preserve">D216</t>
   </si>
   <si>
+    <t xml:space="preserve">D217</t>
+  </si>
+  <si>
     <t xml:space="preserve">D218</t>
   </si>
   <si>
@@ -144,9 +147,6 @@
     <t xml:space="preserve">D226</t>
   </si>
   <si>
-    <t xml:space="preserve">D217</t>
-  </si>
-  <si>
     <t xml:space="preserve">D302</t>
   </si>
   <si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t xml:space="preserve">Classroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacity</t>
   </si>
 </sst>
 </file>
@@ -265,17 +262,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -369,33 +386,34 @@
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -403,10 +421,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>60</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -414,10 +432,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>60</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -425,10 +443,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="6" t="n">
         <v>100</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -436,10 +454,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="6" t="n">
         <v>120</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -447,10 +465,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="7" t="n">
         <v>120</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -458,10 +476,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="7" t="n">
         <v>30</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -469,10 +487,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="7" t="n">
         <v>60</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -480,10 +498,10 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="6" t="n">
         <v>60</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -491,10 +509,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="7" t="n">
         <v>50</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -502,10 +520,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="7" t="n">
         <v>60</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -513,10 +531,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="7" t="n">
         <v>60</v>
       </c>
       <c r="C13" s="0" t="n">
@@ -524,10 +542,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="6" t="n">
         <v>300</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -535,10 +553,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="7" t="n">
         <v>100</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -546,10 +564,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="6" t="n">
         <v>90</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -557,10 +575,10 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" s="7" t="n">
         <v>90</v>
       </c>
       <c r="C17" s="0" t="n">
@@ -568,10 +586,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="6" t="n">
         <v>60</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -579,10 +597,10 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="6" t="n">
         <v>60</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -590,10 +608,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="6" t="n">
         <v>60</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -601,10 +619,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="6" t="n">
         <v>60</v>
       </c>
       <c r="C21" s="0" t="n">
@@ -612,10 +630,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="6" t="n">
         <v>60</v>
       </c>
       <c r="C22" s="0" t="n">
@@ -623,10 +641,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="6" t="n">
         <v>30</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -634,10 +652,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="6" t="n">
         <v>30</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -645,10 +663,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="6" t="n">
         <v>30</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -656,10 +674,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" s="7" t="n">
         <v>60</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -667,10 +685,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="6" t="n">
         <v>60</v>
       </c>
       <c r="C27" s="0" t="n">
@@ -678,10 +696,10 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="7" t="n">
         <v>30</v>
       </c>
       <c r="C28" s="0" t="n">
@@ -689,10 +707,10 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="1" t="n">
+      <c r="A29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="7" t="n">
         <v>60</v>
       </c>
       <c r="C29" s="0" t="n">
@@ -700,10 +718,10 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="7" t="n">
         <v>30</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -711,10 +729,10 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="7" t="n">
         <v>60</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -722,10 +740,10 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="7" t="n">
         <v>30</v>
       </c>
       <c r="C32" s="0" t="n">
@@ -733,10 +751,10 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="7" t="n">
         <v>30</v>
       </c>
       <c r="C33" s="0" t="n">
@@ -744,21 +762,21 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="1" t="n">
-        <v>30</v>
+      <c r="B34" s="7" t="n">
+        <v>150</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="7" t="n">
         <v>30</v>
       </c>
       <c r="C35" s="0" t="n">
@@ -766,21 +784,21 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="1" t="n">
-        <v>60</v>
+      <c r="B36" s="7" t="n">
+        <v>30</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="7" t="n">
         <v>60</v>
       </c>
       <c r="C37" s="0" t="n">
@@ -788,21 +806,21 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="1" t="n">
-        <v>150</v>
+      <c r="B38" s="7" t="n">
+        <v>60</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="7" t="n">
         <v>60</v>
       </c>
       <c r="C39" s="0" t="n">
@@ -810,10 +828,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="7" t="n">
         <v>30</v>
       </c>
       <c r="C40" s="0" t="n">
@@ -821,10 +839,10 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="7" t="n">
         <v>60</v>
       </c>
       <c r="C41" s="0" t="n">
@@ -832,10 +850,10 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="7" t="n">
         <v>30</v>
       </c>
       <c r="C42" s="0" t="n">
@@ -843,10 +861,10 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="1" t="n">
+      <c r="B43" s="7" t="n">
         <v>60</v>
       </c>
       <c r="C43" s="0" t="n">
@@ -854,10 +872,10 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="1" t="n">
+      <c r="B44" s="7" t="n">
         <v>30</v>
       </c>
       <c r="C44" s="0" t="n">
@@ -894,122 +912,122 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>47</v>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="10" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="10" t="n">
         <v>180</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="10" t="n">
         <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="10" t="n">
         <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="10" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="10" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="10" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="10" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="10" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="10" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="10" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="5" t="n">
+      <c r="B13" s="10" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="5" t="n">
+      <c r="B14" s="10" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="5" t="n">
+      <c r="B15" s="10" t="n">
         <v>30</v>
       </c>
     </row>

</xml_diff>